<commit_message>
ANA16: Threat Modelling Analysis for Struts has been added
</commit_message>
<xml_diff>
--- a/Accompanying Material/Analysis/Results/Phase 4 Analysis/Struts Vulnerability Manifest.xlsx
+++ b/Accompanying Material/Analysis/Results/Phase 4 Analysis/Struts Vulnerability Manifest.xlsx
@@ -4,36 +4,28 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="20115" windowHeight="9795"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="20115" windowHeight="9795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vulnerability Description" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Vulnerability Description'!$A$1:$D$33</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="87">
   <si>
     <t>Vulnerability</t>
   </si>
   <si>
-    <t>Vulnerability Description</t>
-  </si>
-  <si>
     <t>CVE-2012-4387</t>
   </si>
   <si>
-    <t>CWE-264 Permissions</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Privileges</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> and Access Controls</t>
-  </si>
-  <si>
     <t>CVE-2012-0391</t>
   </si>
   <si>
@@ -146,13 +138,180 @@
   </si>
   <si>
     <t>CVE-2010-1622</t>
+  </si>
+  <si>
+    <t>CWE-264 Permissions, Privileges and Access Controls</t>
+  </si>
+  <si>
+    <t>Information disclosure</t>
+  </si>
+  <si>
+    <t>Tampering (DoS attack)</t>
+  </si>
+  <si>
+    <t>Tampering (CSRF)</t>
+  </si>
+  <si>
+    <t>Tampering</t>
+  </si>
+  <si>
+    <t>STRIDE Category</t>
+  </si>
+  <si>
+    <t>Threat</t>
+  </si>
+  <si>
+    <t>Identified Vulnerabilities</t>
+  </si>
+  <si>
+    <t>Spoofing the Browser External Entity</t>
+  </si>
+  <si>
+    <t>Cross Site Scripting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elevation Using Impersonation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoofing the Web Server Process </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential Lack of Input Validation for Web Server </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential Data Repudiation by Web Server </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Flow Sniffing </t>
+  </si>
+  <si>
+    <t>Potential Process Crash or Stop for Web Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Flow HTTP Is Potentially Interrupted </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Server May be Subject to Elevation of Privilege Using Remote Code Execution </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elevation by Changing the Execution Flow in Web Server </t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>CVE-2001-1772
+CVE-2011-2087
+CVE-2012-1007</t>
+  </si>
+  <si>
+    <t>CVE-2011-5057
+CVE-2011-0392
+CVE-2012-0393
+CVE-2012-4387
+CVE-2013-0248
+CVE-2013-4152
+CVE-2013-4310
+CVE-2013-6429
+CVE-2013-7315</t>
+  </si>
+  <si>
+    <t>CVE-2008-6504
+CVE-2012-0391
+CVE-2012-0838
+CVE-2013-2248
+CVE-2013-2251</t>
+  </si>
+  <si>
+    <t>Elevation of Privilege / Tampering</t>
+  </si>
+  <si>
+    <t>Elevation of Privilege</t>
+  </si>
+  <si>
+    <t>Tampering / Elevation of Privilege / Information Disclosure</t>
+  </si>
+  <si>
+    <t>Vulnerability CWE</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Does not properly restrict access to collections such as the session and request collections</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to execute arbitrary commands via a crafted HTTP Cookie header that triggers Java code execution through a static method</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to create or overwrite arbitrary files via a crafted parameter that triggers the creation of a Java object</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to cause a denial of service</t>
+  </si>
+  <si>
+    <t>Allows local users to overwrite arbitrary files via an unspecified symlink attack</t>
+  </si>
+  <si>
+    <t>Allows context-dependent attackers to read arbitrary files, cause a denial of service, and conduct CSRF attacks</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to bypass access controls via a crafted action</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to read arbitrary files, cause a denial of service, and conduct CSRF attacks via crafted XML</t>
+  </si>
+  <si>
+    <t>Allows context-dependent attackers to read arbitrary files, cause a denial of service, and conduct CSRF attacks via crafted XML with JAXB</t>
+  </si>
+  <si>
+    <t>CVE-2006-6916
+CVE-2013-6429
+CVE-2007-0185
+CVE-2013-4152
+CVE-2013-7315</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to execute arbitrary code via an HTTP request</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to execute arbitrary commands via unspecified vectors</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to execute arbitrary OGNL code via a crafted parameter name</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to execute arbitrary OGNL code via a crafted request</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to execute arbitrary OGNL code via a request</t>
+  </si>
+  <si>
+    <t>Allows remote attackers to execute arbitrary OGNL code via a request with a crafted value</t>
+  </si>
+  <si>
+    <t>CVE-2012-0392
+CVE-2010-1622
+CVE-2012-0394
+CVE-2013-1965
+CVE-2013-1966
+CVE-2013-2115
+CVE-2013-2134
+CVE-2013-2135</t>
+  </si>
+  <si>
+    <t>Allows attackers to obtain unauthorized access to public methods via a crafted request</t>
+  </si>
+  <si>
+    <t>CVE-2013-4310
+CVE-2007-0184</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +447,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -470,7 +636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -585,6 +751,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -630,8 +861,35 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -974,336 +1232,558 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B13" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="20" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B22" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B26" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D26" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B31" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D33">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Elevation of Privilege"/>
+        <filter val="Elevation of Privilege / Tampering"/>
+        <filter val="Tampering / Elevation of Privilege / Information Disclosure"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="A1:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" t="s">
-        <v>15</v>
+    </row>
+    <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>